<commit_message>
Updated scrum log from yesterday, updated Burndown chart from today
</commit_message>
<xml_diff>
--- a/admin/6-JulSprintBurndown.xlsx
+++ b/admin/6-JulSprintBurndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A15E09-7CFF-4824-9F6B-AE2266B94749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7E9992-161C-46B8-B930-F72CC620C69A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="-16440" windowWidth="29280" windowHeight="16680" xr2:uid="{E7DD3797-FEF2-40B3-90F6-28EA74433530}"/>
+    <workbookView xWindow="13935" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{E7DD3797-FEF2-40B3-90F6-28EA74433530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,10 +526,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,7 +1639,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1790,11 +1790,11 @@
         <v>0</v>
       </c>
       <c r="D11" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="7">
         <f>$B$4-SUM($D$7:D11)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="E12" s="7">
         <f>$B$4-SUM($D$7:D12)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" ref="E14" si="1">E7-E12</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>